<commit_message>
Atualizando dados de vendas
</commit_message>
<xml_diff>
--- a/data/bd_empreendimento.xlsx
+++ b/data/bd_empreendimento.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29728"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="164" documentId="11_92485C45C1F39E42E268565A893E8C18510380CC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{196DEC18-4471-4045-9943-D4946F28A870}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="11_92485C45C1F39E42E268565A893E8C18510380CC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59253780-27C8-404A-BB18-0FF5FC84F2EF}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produtos" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
   <si>
     <t xml:space="preserve">id_produto
 </t>
@@ -74,6 +74,18 @@
     <t>Sim</t>
   </si>
   <si>
+    <t>P002</t>
+  </si>
+  <si>
+    <t>P003</t>
+  </si>
+  <si>
+    <t>P004</t>
+  </si>
+  <si>
+    <t>P005</t>
+  </si>
+  <si>
     <t>Id_venda</t>
   </si>
   <si>
@@ -107,6 +119,24 @@
     <t>Enviado</t>
   </si>
   <si>
+    <t>V002</t>
+  </si>
+  <si>
+    <t>V003</t>
+  </si>
+  <si>
+    <t>V004</t>
+  </si>
+  <si>
+    <t>V005</t>
+  </si>
+  <si>
+    <t>Mercado Livre</t>
+  </si>
+  <si>
+    <t>Em Produção</t>
+  </si>
+  <si>
     <t>estoque_inicial</t>
   </si>
   <si>
@@ -138,6 +168,21 @@
   </si>
   <si>
     <t>Vela Lavanda</t>
+  </si>
+  <si>
+    <t>C002</t>
+  </si>
+  <si>
+    <t>C003</t>
+  </si>
+  <si>
+    <t>C004</t>
+  </si>
+  <si>
+    <t>C005</t>
+  </si>
+  <si>
+    <t>Jornal Pet</t>
   </si>
   <si>
     <t>ano</t>
@@ -204,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -231,6 +276,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,8 +508,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C4D27FB-D767-4F7A-BE7F-1EC368D4E5F9}" name="Tabela1" displayName="Tabela1" ref="A1:G2" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
-  <autoFilter ref="A1:G2" xr:uid="{3C4D27FB-D767-4F7A-BE7F-1EC368D4E5F9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C4D27FB-D767-4F7A-BE7F-1EC368D4E5F9}" name="Tabela1" displayName="Tabela1" ref="A1:G6" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+  <autoFilter ref="A1:G6" xr:uid="{3C4D27FB-D767-4F7A-BE7F-1EC368D4E5F9}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{53854E17-1025-4318-A11A-EB722F5127A7}" name="id_produto_x000a_" dataDxfId="38"/>
     <tableColumn id="2" xr3:uid="{6BFED019-13AD-45B5-A924-A9DDD102D935}" name="nome_Produto" dataDxfId="37"/>
@@ -475,8 +524,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CEA61A6E-7503-475A-B94D-40013691D3DF}" name="Tabela2" displayName="Tabela2" ref="A1:H2" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:H2" xr:uid="{CEA61A6E-7503-475A-B94D-40013691D3DF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CEA61A6E-7503-475A-B94D-40013691D3DF}" name="Tabela2" displayName="Tabela2" ref="A1:H6" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A1:H6" xr:uid="{CEA61A6E-7503-475A-B94D-40013691D3DF}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{EEF109AB-A9A5-4BE0-A26A-E3CB512E6A00}" name="Id_venda" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{61968229-18BB-4F50-BD3C-7273F225B879}" name="data" dataDxfId="28"/>
@@ -492,15 +541,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{904FB13F-0ADA-4C85-8632-579495880D14}" name="Tabela3" displayName="Tabela3" ref="A1:E2" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:E2" xr:uid="{904FB13F-0ADA-4C85-8632-579495880D14}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{904FB13F-0ADA-4C85-8632-579495880D14}" name="Tabela3" displayName="Tabela3" ref="A1:E6" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:E6" xr:uid="{904FB13F-0ADA-4C85-8632-579495880D14}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{70C0DD3A-C2E9-4814-9FA1-F1FE119E438B}" name="id_produto" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{EB25A646-0A47-4126-82B3-2F2192643A87}" name="estoque_inicial" dataDxfId="18"/>
     <tableColumn id="3" xr3:uid="{0C91F562-21E7-4F3E-A157-62DB82EE95D7}" name="entradas" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{42EC167D-F349-4EF9-BC91-FCE35B9B9DC5}" name="saidas" dataDxfId="16">
-      <calculatedColumnFormula>SUMIF(Vendas!D2, Vendas!E2)</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="4" xr3:uid="{42EC167D-F349-4EF9-BC91-FCE35B9B9DC5}" name="saidas" dataDxfId="16"/>
     <tableColumn id="5" xr3:uid="{FD2E2D18-5250-4776-9677-77706527BFDD}" name="ponto_reposicao" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -508,8 +555,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7593D0EA-79CB-4760-A2B4-4F4F32B06E34}" name="Tabela4" displayName="Tabela4" ref="A1:E2" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:E2" xr:uid="{7593D0EA-79CB-4760-A2B4-4F4F32B06E34}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7593D0EA-79CB-4760-A2B4-4F4F32B06E34}" name="Tabela4" displayName="Tabela4" ref="A1:E6" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:E6" xr:uid="{7593D0EA-79CB-4760-A2B4-4F4F32B06E34}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{E3FD224A-30BB-49BC-9F83-C3113CA17136}" name="id_custo" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{391930BC-CAA2-4EE3-8808-5BDF666CD2CB}" name="tipo_custo" dataDxfId="11"/>
@@ -833,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.7109375" defaultRowHeight="15"/>
@@ -893,8 +940,103 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4">
+        <v>35</v>
+      </c>
+      <c r="F3" s="4">
+        <v>119</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4">
+        <v>35</v>
+      </c>
+      <c r="F4" s="4">
+        <v>119</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4">
+        <v>35</v>
+      </c>
+      <c r="F5" s="4">
+        <v>119</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="4">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4">
+        <v>60</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="8" spans="1:7">
       <c r="D8" s="7"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -906,49 +1048,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711F28CF-294D-42AB-BB50-337B69AF1278}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B2" s="5">
         <v>46054</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -960,11 +1102,118 @@
         <v>119</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="5">
+        <v>46055</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>119</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="5">
+        <v>46056</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>119</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5">
+        <v>46057</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>119</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5">
+        <v>46058</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4">
+        <v>60</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="G10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -976,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5A7221-259C-435C-A626-1E27A639FBE6}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="15"/>
@@ -989,19 +1238,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1015,12 +1264,82 @@
         <v>10</v>
       </c>
       <c r="D2" s="6">
-        <f>SUMIF(Vendas!D2, Vendas!E2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3">
         <v>5</v>
       </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="D11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1032,47 +1351,118 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD1EC00-10A8-42CB-ABD8-9EE96687F3BB}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D2" s="4">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" s="5">
         <v>46054</v>
       </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4">
+        <v>119</v>
+      </c>
+      <c r="E3" s="5">
+        <v>46055</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="4">
+        <v>119</v>
+      </c>
+      <c r="E4" s="5">
+        <v>46056</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4">
+        <v>119</v>
+      </c>
+      <c r="E5" s="5">
+        <v>46057</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="4">
+        <v>60</v>
+      </c>
+      <c r="E6" s="5">
+        <v>46058</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1087,29 +1477,29 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1121,7 +1511,7 @@
       <c r="F2" s="3"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="C7" s="9"/>
+      <c r="C7" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>